<commit_message>
if the relevant property is 1=2 (processedByMirth) the field will never be created on the ODK collect Output.
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/DEATHTOHOH.xlsx
+++ b/xforms/xlsforms/DEATHTOHOH.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="126">
   <si>
     <t>type</t>
   </si>
@@ -300,9 +300,6 @@
     <t>processedByMirth</t>
   </si>
   <si>
-    <t>1=2</t>
-  </si>
-  <si>
     <t>bywho</t>
   </si>
   <si>
@@ -391,9 +388,6 @@
   </si>
   <si>
     <t>Kwingine</t>
-  </si>
-  <si>
-    <t>pbm</t>
   </si>
   <si>
     <t>householdId</t>
@@ -1601,10 +1595,10 @@
   <dimension ref="A1:P64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1809,10 +1803,10 @@
         <v>21</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H9" s="4" t="b">
         <v>1</v>
@@ -2070,14 +2064,11 @@
       <c r="B24" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="D24" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>125</v>
+        <v>93</v>
+      </c>
+      <c r="K24" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
@@ -2282,240 +2273,240 @@
     </row>
     <row r="10" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="15">
+        <v>1</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="15">
-        <v>1</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>96</v>
-      </c>
       <c r="D10" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="15">
         <v>2</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="15">
         <v>3</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="15">
         <v>4</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>101</v>
-      </c>
       <c r="C14" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>103</v>
-      </c>
       <c r="D15" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>106</v>
-      </c>
       <c r="D17" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="C23" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>114</v>
-      </c>
       <c r="D23" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2526,10 +2517,10 @@
         <v>31</v>
       </c>
       <c r="C27" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2540,10 +2531,10 @@
         <v>32</v>
       </c>
       <c r="C28" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="16" t="s">
         <v>117</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2551,13 +2542,13 @@
         <v>88</v>
       </c>
       <c r="B29" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C29" s="16" t="s">
-        <v>120</v>
-      </c>
       <c r="D29" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2565,13 +2556,13 @@
         <v>88</v>
       </c>
       <c r="B30" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C30" s="16" t="s">
-        <v>122</v>
-      </c>
       <c r="D30" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2579,13 +2570,13 @@
         <v>88</v>
       </c>
       <c r="B31" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C31" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="D31" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modified Death of HoH form to concat place of death
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/DEATHTOHOH.xlsx
+++ b/xforms/xlsforms/DEATHTOHOH.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="225" windowWidth="21600" windowHeight="9900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="285" windowWidth="21600" windowHeight="9840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="130">
   <si>
     <t>type</t>
   </si>
@@ -394,6 +394,18 @@
   </si>
   <si>
     <t>HouseHoldId</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>causeOfDeath</t>
+  </si>
+  <si>
+    <t>Cause of death</t>
+  </si>
+  <si>
+    <t>concat(${causeofdeathdiagnosed},${causofdeathnotdiagnosed})</t>
   </si>
 </sst>
 </file>
@@ -1592,13 +1604,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P64"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K24" sqref="K24"/>
+      <selection pane="bottomRight" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1941,57 +1953,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="K17" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="5" t="b">
+      <c r="C18" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K17" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="H18" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="P18" s="5" t="s">
+      <c r="P19" s="5" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="H19" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K19" s="5" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
@@ -1999,10 +2009,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -2014,14 +2024,14 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -2032,50 +2042,66 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>42</v>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="H22" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="D23" s="9"/>
+      <c r="K22" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
+      <c r="H23" s="5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="K24" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H25" s="3"/>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H33" s="3"/>
+      <c r="K25" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H26" s="3"/>
     </row>
     <row r="34" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H34" s="3"/>
@@ -2089,8 +2115,8 @@
     <row r="37" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H37" s="3"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H54" s="3"/>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H38" s="3"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H55" s="3"/>
@@ -2105,7 +2131,6 @@
       <c r="H58" s="3"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="3"/>
       <c r="H59" s="3"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -2117,10 +2142,14 @@
       <c r="H61" s="3"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="3"/>
       <c r="H62" s="3"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H64" s="3"/>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H63" s="3"/>
+    </row>
+    <row r="65" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H65" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Slightly ajusted some core event form field positions/labels
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/DEATHTOHOH.xlsx
+++ b/xforms/xlsforms/DEATHTOHOH.xlsx
@@ -141,12 +141,6 @@
     <t>Outcomes</t>
   </si>
   <si>
-    <t>Social Group Id</t>
-  </si>
-  <si>
-    <t>Relationship to Group Head</t>
-  </si>
-  <si>
     <t>Brother/Sister</t>
   </si>
   <si>
@@ -207,9 +201,6 @@
     <t>Membership</t>
   </si>
   <si>
-    <t>Member Id</t>
-  </si>
-  <si>
     <t>hh_people_nb</t>
   </si>
   <si>
@@ -219,9 +210,6 @@
     <t>new_hoh_id</t>
   </si>
   <si>
-    <t>New Hoh Id</t>
-  </si>
-  <si>
     <t>memberName</t>
   </si>
   <si>
@@ -231,9 +219,6 @@
     <t>individualId</t>
   </si>
   <si>
-    <t>Individual ID</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -255,9 +240,6 @@
     <t>whom</t>
   </si>
   <si>
-    <t>by whom?</t>
-  </si>
-  <si>
     <t>selected(${diagnoseddeath}, '1')</t>
   </si>
   <si>
@@ -393,9 +375,6 @@
     <t>householdId</t>
   </si>
   <si>
-    <t>HouseHoldId</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -406,6 +385,27 @@
   </si>
   <si>
     <t>concat(${causeofdeathdiagnosed},${causofdeathnotdiagnosed})</t>
+  </si>
+  <si>
+    <t>Individual ID of deceased HOH</t>
+  </si>
+  <si>
+    <t>Individual ID of the NEW Head of Household</t>
+  </si>
+  <si>
+    <t>Social Group ID</t>
+  </si>
+  <si>
+    <t>Who diagnosed the cause of death?</t>
+  </si>
+  <si>
+    <t>Member ID</t>
+  </si>
+  <si>
+    <t>Relationship to NEW Social Group Head</t>
+  </si>
+  <si>
+    <t>processed</t>
   </si>
 </sst>
 </file>
@@ -1607,10 +1607,10 @@
   <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1676,7 +1676,7 @@
         <v>13</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -1764,10 +1764,10 @@
         <v>21</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="H6" s="4" t="b">
         <v>1</v>
@@ -1781,10 +1781,10 @@
         <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>67</v>
+        <v>124</v>
       </c>
       <c r="H7" s="4" t="b">
         <v>1</v>
@@ -1815,7 +1815,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>125</v>
@@ -1829,13 +1829,13 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H10" s="5" t="b">
         <v>1</v>
@@ -1843,13 +1843,13 @@
     </row>
     <row r="11" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -1861,16 +1861,16 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -1882,16 +1882,16 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1903,16 +1903,16 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H15" s="5" t="b">
         <v>1</v>
@@ -1941,13 +1941,13 @@
         <v>21</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H16" s="5" t="b">
         <v>1</v>
@@ -1955,16 +1955,16 @@
     </row>
     <row r="17" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="K17" s="5" t="b">
         <v>1</v>
@@ -1972,10 +1972,10 @@
     </row>
     <row r="18" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>0</v>
@@ -1992,16 +1992,16 @@
     </row>
     <row r="19" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="P19" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="P19" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
@@ -2009,10 +2009,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>63</v>
+        <v>127</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -2028,10 +2028,10 @@
         <v>21</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -2050,7 +2050,7 @@
         <v>23</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -2063,13 +2063,13 @@
     </row>
     <row r="23" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>42</v>
+        <v>128</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -2079,7 +2079,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B24" s="2"/>
       <c r="D24" s="9"/>
@@ -2088,13 +2088,13 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="K25" s="5" t="b">
         <v>1</v>
@@ -2199,7 +2199,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2213,7 +2213,7 @@
         <v>26</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2227,7 +2227,7 @@
         <v>27</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2255,7 +2255,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2269,7 +2269,7 @@
         <v>30</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2302,310 +2302,310 @@
     </row>
     <row r="10" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B10" s="15">
         <v>1</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B11" s="15">
         <v>2</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B12" s="15">
         <v>3</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B13" s="15">
         <v>4</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>105</v>
-      </c>
       <c r="D17" s="15" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2691,24 +2691,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
         <v>54</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated OpenHDS Mobile and Forms to work with issue https://github.com/SwissTPH/openhds-tablet/issues/7
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/DEATHTOHOH.xlsx
+++ b/xforms/xlsforms/DEATHTOHOH.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="139">
   <si>
     <t>type</t>
   </si>
@@ -406,6 +406,33 @@
   </si>
   <si>
     <t>processed</t>
+  </si>
+  <si>
+    <t>begin group</t>
+  </si>
+  <si>
+    <t>openhds</t>
+  </si>
+  <si>
+    <t>OpenHDS preloaded info</t>
+  </si>
+  <si>
+    <t>end group</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>First name of deceased HOH</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>Last name of deceased HOH</t>
+  </si>
+  <si>
+    <t>field-list</t>
   </si>
 </sst>
 </file>
@@ -485,7 +512,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -495,6 +522,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -861,7 +894,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -916,6 +949,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1604,13 +1643,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1742,49 +1781,54 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" s="5" t="b">
-        <v>1</v>
-      </c>
+    <row r="5" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="J5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
     </row>
     <row r="6" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>123</v>
+        <v>38</v>
       </c>
       <c r="H6" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="K6" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K6" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>124</v>
+        <v>39</v>
       </c>
       <c r="H7" s="4" t="b">
         <v>1</v>
@@ -1798,10 +1842,10 @@
         <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>39</v>
+        <v>125</v>
       </c>
       <c r="H8" s="4" t="b">
         <v>1</v>
@@ -1810,346 +1854,402 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H9" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="K9" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K9" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>67</v>
+        <v>134</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="K10" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="K11" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>124</v>
+      </c>
       <c r="H12" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="4"/>
+      <c r="K12" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="H13" s="22"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B18" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H15" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="H19" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="H16" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="H20" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J21" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="K17" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="K21" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="5" t="b">
+      <c r="C22" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K18" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+      <c r="H22" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="P19" s="5" t="s">
+      <c r="P23" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B24" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D24" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="H20" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K20" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="H21" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K21" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="H22" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K22" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="H23" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="D24" s="9"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
+      <c r="H24" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" s="5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="H25" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="H26" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="H27" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="K25" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H26" s="3"/>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H37" s="3"/>
+      <c r="K29" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H30" s="3"/>
     </row>
     <row r="38" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H38" s="3"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H55" s="3"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H56" s="3"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H57" s="3"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H58" s="3"/>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H39" s="3"/>
+    </row>
+    <row r="40" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H42" s="3"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H59" s="3"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
       <c r="H60" s="3"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
       <c r="H61" s="3"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="3"/>
       <c r="H62" s="3"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H63" s="3"/>
     </row>
-    <row r="65" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="3"/>
+      <c r="H64" s="3"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="3"/>
       <c r="H65" s="3"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="3"/>
+      <c r="H66" s="3"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H67" s="3"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H69" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>